<commit_message>
update some .v unit
</commit_message>
<xml_diff>
--- a/cpu部件.xlsx
+++ b/cpu部件.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86152\Desktop\cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A136E7CF-9679-4671-A226-D74235FD27B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1C09E5-8C26-461E-B4C9-53795E82470D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{7A3390E4-5CD4-4269-B22F-F864EC2D77B9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="76">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,6 +170,158 @@
   </si>
   <si>
     <t>srav</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MUX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MUX_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF.RD1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC+4&amp;RF.RD1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXT16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC+4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMEM[15:0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addiu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>andi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMEM[15:0](无符号)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ori</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xori</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DMEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF.RD2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>beq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EXT18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMEM[15:0] || 00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bne</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sltiu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>j</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>||</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC[31:28]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMEM[25:0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC+4 : ||</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -224,7 +376,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -232,12 +384,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -554,46 +715,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C28C2FB-382E-4B7F-9395-01D8A7787FB0}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="8.88671875" style="7"/>
+    <col min="17" max="17" width="11.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3" t="s">
+      <c r="I1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="6"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
@@ -602,10 +789,31 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -625,7 +833,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -645,7 +853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -665,7 +873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -685,7 +893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -705,7 +913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -725,7 +933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -745,7 +953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -765,7 +973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -776,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -788,7 +996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -799,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -811,7 +1019,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -834,7 +1042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -857,7 +1065,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -880,7 +1088,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -903,7 +1111,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -926,32 +1134,392 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="J28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+      <c r="K32" t="s">
+        <v>75</v>
+      </c>
+      <c r="N32" t="s">
+        <v>41</v>
+      </c>
+      <c r="O32">
+        <v>8</v>
+      </c>
+      <c r="P32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>